<commit_message>
Jurisdiction with Different Users
</commit_message>
<xml_diff>
--- a/Lexis-GLOBAL/Coredata/JURISDICTION.xlsx
+++ b/Lexis-GLOBAL/Coredata/JURISDICTION.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adapp\git\RestAssured\Lexis-GLOBAL\Coredata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adapp\git\AutoAPI\Lexis-GLOBAL\Coredata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFEAED6-4C8E-4B96-B5FA-E1D1F0DCE476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE98FF6-E612-418C-8E88-4632BA2DDD6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="54">
   <si>
     <t>Description</t>
   </si>
@@ -146,6 +146,51 @@
   </si>
   <si>
     <t>api/v1/UserJurisdiction</t>
+  </si>
+  <si>
+    <t>RegionalAdmin</t>
+  </si>
+  <si>
+    <t>CompanyAdmin</t>
+  </si>
+  <si>
+    <t>AccountIT</t>
+  </si>
+  <si>
+    <t>Approver</t>
+  </si>
+  <si>
+    <t>NormalUser</t>
+  </si>
+  <si>
+    <t>Valid_RegionalUsername</t>
+  </si>
+  <si>
+    <t>Valid_RegionalPassword</t>
+  </si>
+  <si>
+    <t>Valid_CompanyAdminUsername</t>
+  </si>
+  <si>
+    <t>Valid_CompanyAdminPassword</t>
+  </si>
+  <si>
+    <t>Valid_AccountITUsername</t>
+  </si>
+  <si>
+    <t>Valid_AccountITPassword</t>
+  </si>
+  <si>
+    <t>Valid_ApproverUsername</t>
+  </si>
+  <si>
+    <t>Valid_ApproverPassword</t>
+  </si>
+  <si>
+    <t>Valid_NormalUsername</t>
+  </si>
+  <si>
+    <t>Valid_NormalPassword</t>
   </si>
 </sst>
 </file>
@@ -191,7 +236,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -214,11 +259,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -237,6 +295,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,26 +587,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="13.26953125" customWidth="1"/>
     <col min="3" max="3" width="11.08984375" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" customWidth="1"/>
     <col min="5" max="5" width="20.7265625" customWidth="1"/>
     <col min="6" max="6" width="19.54296875" customWidth="1"/>
     <col min="7" max="7" width="17.90625" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
     <col min="9" max="9" width="17.1796875" customWidth="1"/>
     <col min="10" max="10" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="10.81640625" customWidth="1"/>
-    <col min="17" max="17" width="21.81640625" customWidth="1"/>
-    <col min="18" max="18" width="19.6328125" customWidth="1"/>
+    <col min="11" max="16" width="10.81640625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="29.6328125" customWidth="1"/>
+    <col min="18" max="18" width="27.90625" customWidth="1"/>
     <col min="19" max="19" width="9.81640625" customWidth="1"/>
     <col min="20" max="20" width="15.453125" customWidth="1"/>
   </cols>
@@ -605,7 +674,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A2" s="4">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -614,7 +683,7 @@
       <c r="C2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -664,8 +733,305 @@
       </c>
       <c r="T2" s="3"/>
     </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T3" s="8"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T4" s="8"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T5" s="8"/>
+    </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="H6" s="3"/>
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T6" s="8"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T7" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -675,25 +1041,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ACB960E-223F-4AE9-98CE-ED5CFAD5DF6F}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="S2" sqref="S2:S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="13.54296875" customWidth="1"/>
     <col min="3" max="3" width="11.08984375" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" customWidth="1"/>
     <col min="5" max="5" width="19.90625" customWidth="1"/>
     <col min="6" max="6" width="19.54296875" customWidth="1"/>
     <col min="7" max="7" width="17.90625" customWidth="1"/>
     <col min="8" max="9" width="17.7265625" customWidth="1"/>
     <col min="10" max="10" width="17.81640625" customWidth="1"/>
-    <col min="11" max="16" width="17.7265625" customWidth="1"/>
-    <col min="17" max="17" width="21.81640625" customWidth="1"/>
-    <col min="18" max="18" width="19.6328125" customWidth="1"/>
+    <col min="11" max="16" width="17.7265625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="31.08984375" customWidth="1"/>
+    <col min="18" max="18" width="29" customWidth="1"/>
     <col min="19" max="19" width="9.81640625" customWidth="1"/>
     <col min="20" max="20" width="15.453125" customWidth="1"/>
     <col min="22" max="22" width="11.81640625" customWidth="1"/>
@@ -821,6 +1187,306 @@
       </c>
       <c r="T2" s="3"/>
     </row>
+    <row r="3" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T3" s="3"/>
+    </row>
+    <row r="4" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T4" s="3"/>
+    </row>
+    <row r="5" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T5" s="3"/>
+    </row>
+    <row r="6" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T6" s="3"/>
+    </row>
+    <row r="7" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T7" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -829,26 +1495,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F95895-1565-490A-84F8-C69F3E6A01E3}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="S3" activeCellId="1" sqref="S2 S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="13.26953125" customWidth="1"/>
     <col min="3" max="3" width="11.08984375" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
     <col min="5" max="6" width="19.453125" customWidth="1"/>
     <col min="7" max="7" width="12.54296875" customWidth="1"/>
     <col min="8" max="8" width="16.6328125" customWidth="1"/>
     <col min="9" max="9" width="15.7265625" customWidth="1"/>
     <col min="10" max="10" width="17.36328125" customWidth="1"/>
     <col min="11" max="11" width="17.54296875" customWidth="1"/>
-    <col min="12" max="16" width="16.26953125" customWidth="1"/>
-    <col min="17" max="17" width="21.81640625" customWidth="1"/>
-    <col min="18" max="18" width="19.6328125" customWidth="1"/>
+    <col min="12" max="16" width="16.26953125" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="30.6328125" customWidth="1"/>
+    <col min="18" max="18" width="28.36328125" customWidth="1"/>
     <col min="19" max="19" width="9.81640625" customWidth="1"/>
     <col min="20" max="20" width="15.453125" customWidth="1"/>
   </cols>
@@ -915,8 +1581,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="4">
+    <row r="2" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -974,6 +1640,360 @@
         <v>16</v>
       </c>
       <c r="T2" s="3"/>
+    </row>
+    <row r="3" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T3" s="8"/>
+    </row>
+    <row r="4" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T4" s="8"/>
+    </row>
+    <row r="5" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T5" s="8"/>
+    </row>
+    <row r="6" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T6" s="8"/>
+    </row>
+    <row r="7" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T7" s="8"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="K10" s="11"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="K11" s="11"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="K12" s="11"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="K13" s="11"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="K14" s="11"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="K15" s="11"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="K16" s="11"/>
+    </row>
+    <row r="17" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K17" s="11"/>
+    </row>
+    <row r="18" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K18" s="11"/>
+    </row>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K19" s="11"/>
+    </row>
+    <row r="20" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K20" s="11"/>
+    </row>
+    <row r="21" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K21" s="11"/>
+    </row>
+    <row r="22" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K22" s="11"/>
+    </row>
+    <row r="23" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K23" s="11"/>
+    </row>
+    <row r="24" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K24" s="11"/>
+    </row>
+    <row r="25" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K25" s="11"/>
+    </row>
+    <row r="26" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K26" s="11"/>
+    </row>
+    <row r="27" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K27" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -982,25 +2002,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E893E9-EC4B-4E3D-B472-D440A1662D77}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="13.26953125" customWidth="1"/>
     <col min="3" max="3" width="11.08984375" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="19.54296875" customWidth="1"/>
     <col min="7" max="7" width="14.81640625" customWidth="1"/>
     <col min="8" max="8" width="16.54296875" customWidth="1"/>
     <col min="9" max="9" width="16.6328125" customWidth="1"/>
-    <col min="10" max="16" width="10.81640625" customWidth="1"/>
-    <col min="17" max="17" width="21.81640625" customWidth="1"/>
-    <col min="18" max="18" width="19.6328125" customWidth="1"/>
+    <col min="10" max="16" width="10.81640625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="29.08984375" customWidth="1"/>
+    <col min="18" max="18" width="28.08984375" customWidth="1"/>
     <col min="19" max="19" width="9.81640625" customWidth="1"/>
     <col min="20" max="20" width="15.453125" customWidth="1"/>
   </cols>
@@ -1071,13 +2091,13 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -1126,6 +2146,306 @@
         <v>16</v>
       </c>
       <c r="T2" s="3"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T3" s="3"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T4" s="3"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T5" s="3"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T6" s="3"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1134,25 +2454,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E89AE917-7A58-49C0-9ED9-4EEA5D928C77}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="13.26953125" customWidth="1"/>
     <col min="3" max="3" width="11.08984375" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="4" max="4" width="14.36328125" customWidth="1"/>
     <col min="5" max="5" width="20.7265625" customWidth="1"/>
     <col min="6" max="6" width="19.54296875" customWidth="1"/>
     <col min="7" max="7" width="17.90625" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
     <col min="9" max="9" width="17.1796875" customWidth="1"/>
-    <col min="10" max="16" width="10.81640625" customWidth="1"/>
-    <col min="17" max="17" width="21.81640625" customWidth="1"/>
-    <col min="18" max="18" width="19.6328125" customWidth="1"/>
+    <col min="10" max="16" width="10.81640625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="29.81640625" customWidth="1"/>
+    <col min="18" max="18" width="29.453125" customWidth="1"/>
     <col min="19" max="19" width="9.81640625" customWidth="1"/>
     <col min="20" max="20" width="15.453125" customWidth="1"/>
   </cols>
@@ -1220,7 +2540,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A2" s="4">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1229,7 +2549,7 @@
       <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -1278,6 +2598,306 @@
         <v>16</v>
       </c>
       <c r="T2" s="3"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T3" s="3"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T4" s="3"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T5" s="3"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T6" s="3"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Jurisdiction in term of Different User and Integration flow
</commit_message>
<xml_diff>
--- a/Lexis-GLOBAL/Coredata/JURISDICTION.xlsx
+++ b/Lexis-GLOBAL/Coredata/JURISDICTION.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adapp\git\AutoAPI\Lexis-GLOBAL\Coredata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE98FF6-E612-418C-8E88-4632BA2DDD6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EFDC27-4CEB-40AA-952C-A5E7F254884C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction_Create" sheetId="1" r:id="rId1"/>
@@ -589,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -735,7 +735,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>18</v>
@@ -795,7 +795,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>18</v>
@@ -855,7 +855,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>18</v>
@@ -915,7 +915,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>18</v>
@@ -975,7 +975,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>18</v>
@@ -1043,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ACB960E-223F-4AE9-98CE-ED5CFAD5DF6F}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:S3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5:S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1497,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F95895-1565-490A-84F8-C69F3E6A01E3}">
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S3" activeCellId="1" sqref="S2 S3"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2004,8 +2004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E893E9-EC4B-4E3D-B472-D440A1662D77}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2456,8 +2456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E89AE917-7A58-49C0-9ED9-4EEA5D928C77}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>